<commit_message>
Optimising the framework with merging import statements and Code
</commit_message>
<xml_diff>
--- a/target/test-classes/TutorialsNinjaData.xlsx
+++ b/target/test-classes/TutorialsNinjaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_Workspace\LiveAutomationProject_TN\LiveAutomationProject_TutorialsNinja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C15D03-B3E4-452C-BB38-667D266878D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD832A4-0AD0-4FAB-BEEE-6BBA1DC9631E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>RegisterTestsSupplyPasswords</t>
   </si>
   <si>
-    <t>Passwords</t>
-  </si>
-  <si>
     <t>abcdefg</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>ABCD123#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -428,22 +428,22 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new Class ElementsUtilities.java and modify framework
</commit_message>
<xml_diff>
--- a/target/test-classes/TutorialsNinjaData.xlsx
+++ b/target/test-classes/TutorialsNinjaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse_Workspace\LiveAutomationProject_TN\LiveAutomationProject_TutorialsNinja\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C15D03-B3E4-452C-BB38-667D266878D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD832A4-0AD0-4FAB-BEEE-6BBA1DC9631E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>RegisterTestsSupplyPasswords</t>
   </si>
   <si>
-    <t>Passwords</t>
-  </si>
-  <si>
     <t>abcdefg</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>ABCD123#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E7:E8"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -428,22 +428,22 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>